<commit_message>
Modify the original data table style
修改原始数据表格样式，则，相应的过滤拟合结果样式有所变化
</commit_message>
<xml_diff>
--- a/过滤/原始数据.xlsx
+++ b/过滤/原始数据.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SpyderNow\过滤\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\spyNow\化工原理实验\过滤\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D531E5-CDF9-4A09-8489-F0B9FA87F930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF861C4-AF46-47E7-8FC8-7E979A50BBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{4D78158A-9E1A-48EE-B62C-81AF569EB9F1}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +85,15 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -126,7 +135,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -145,13 +154,16 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -475,7 +487,7 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -487,404 +499,404 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>5</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>0</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>5</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="6">
         <v>0</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="6">
         <v>0</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="5">
         <v>5</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <v>0</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>6</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>17.68</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>17.68</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>6</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>14.6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="6">
         <v>14.6</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>6</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <v>9.0399999999999991</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="6">
         <v>9.0399999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>7</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>57.88</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>40.200000000000003</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>7</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <v>35.61</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="6">
         <v>21.01</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>7</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="6">
         <v>25.7</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="6">
         <v>16.66</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>8</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>117.64</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>59.76</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>8</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="6">
         <v>64.53</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="6">
         <v>28.91</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>8</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <v>48.74</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="6">
         <v>23.04</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>9</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>183.41</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>65.77</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>9</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>94.71</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>30.17</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <v>9</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="6">
         <v>73.95</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="6">
         <v>25.21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>10</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>261.36</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>77.95</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>10</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>135.71</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="6">
         <v>41</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <v>10</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="6">
         <v>106.55</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="6">
         <v>32.6</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>11</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="6">
         <v>359.7</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>98.34</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>11</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="6">
         <v>183.58</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>47.87</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <v>11</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="6">
         <v>141.28</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="6">
         <v>34.729999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>12</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="6">
         <v>470.81</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>111.11</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>12</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="6">
         <v>237.58</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="6">
         <v>53.99</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <v>12</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="6">
         <v>182.11</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="6">
         <v>40.83</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>13</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="6">
         <v>600.73</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>129.91999999999999</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>13</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="6">
         <v>296.64999999999998</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="6">
         <v>59.06</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <v>13</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="6">
         <v>225.95</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="6">
         <v>43.84</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>14</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="6">
         <v>857.51</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="6">
         <v>256.77999999999997</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>14</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="6">
         <v>381.12</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="6">
         <v>84.47</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="5">
         <v>14</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <v>280.95</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="6">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>14.5</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="6">
         <v>3521.72</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>2664.21</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>15</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <v>813.05</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="6">
         <v>431.92</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="5">
         <v>15</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="6">
         <v>401.56</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="6">
         <v>120.61</v>
       </c>
     </row>

</xml_diff>